<commit_message>
docs: finalize docs workflow and help snapshots
</commit_message>
<xml_diff>
--- a/output/xlsx/ready_to_print.xlsx
+++ b/output/xlsx/ready_to_print.xlsx
@@ -438,7 +438,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Generated (MT): 2026-01-09 13:15:50 MT</t>
+          <t>Generated (MT): 2026-01-17 10:47:28 MT</t>
         </is>
       </c>
     </row>
@@ -831,7 +831,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Generated (MT): 2026-01-09 13:15:50 MT</t>
+          <t>Generated (MT): 2026-01-17 10:47:28 MT</t>
         </is>
       </c>
     </row>

</xml_diff>